<commit_message>
done for today, now working to format the excel file
</commit_message>
<xml_diff>
--- a/assets/latest data/Fixed formulas-2.xlsx
+++ b/assets/latest data/Fixed formulas-2.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2. Research\Projects\uvas ttsf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\donewithit\assets\latest data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B2CC139B-3519-D54D-BCD0-C26316F7C375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Test One" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="73">
   <si>
     <t>Barseem and wheat straw based</t>
   </si>
@@ -261,7 +261,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -772,19 +772,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB28"/>
   <sheetViews>
     <sheetView zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
       <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="19.7734375" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -835,7 +835,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -903,7 +903,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="W3" t="s">
         <v>27</v>
       </c>
@@ -911,7 +911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="G4" s="17"/>
       <c r="H4" s="17" t="s">
         <v>16</v>
@@ -959,7 +959,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="G5" t="s">
         <v>24</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="G6" t="s">
         <v>63</v>
       </c>
@@ -1059,7 +1059,7 @@
       </c>
       <c r="X6" s="18"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="G7" t="s">
         <v>25</v>
       </c>
@@ -1115,7 +1115,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="G8" t="s">
         <v>57</v>
       </c>
@@ -1159,7 +1159,7 @@
       </c>
       <c r="X8" s="18"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="G9" t="s">
         <v>26</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="G10" t="s">
         <v>27</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="G11" t="s">
         <v>28</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="G12" t="s">
         <v>64</v>
       </c>
@@ -1364,7 +1364,7 @@
       </c>
       <c r="W12" s="15"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="G13" t="s">
         <v>29</v>
       </c>
@@ -1414,7 +1414,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="G14" t="s">
         <v>30</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>42.5</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="G15" t="s">
         <v>43</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>0.30241599999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="G16" t="s">
         <v>31</v>
       </c>
@@ -1557,7 +1557,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="7:28" x14ac:dyDescent="0.2">
+    <row r="17" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G17" t="s">
         <v>41</v>
       </c>
@@ -1607,7 +1607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="7:28" x14ac:dyDescent="0.2">
+    <row r="18" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G18" t="s">
         <v>32</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="19" spans="7:28" x14ac:dyDescent="0.2">
+    <row r="19" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G19" t="s">
         <v>42</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="7:28" x14ac:dyDescent="0.2">
+    <row r="20" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G20" s="15" t="s">
         <v>33</v>
       </c>
@@ -1759,7 +1759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="7:28" x14ac:dyDescent="0.2">
+    <row r="21" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G21" s="15" t="s">
         <v>34</v>
       </c>
@@ -1809,7 +1809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="7:28" x14ac:dyDescent="0.2">
+    <row r="22" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G22" s="15" t="s">
         <v>35</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="7:28" x14ac:dyDescent="0.2">
+    <row r="23" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G23" s="15" t="s">
         <v>36</v>
       </c>
@@ -1909,7 +1909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="7:28" x14ac:dyDescent="0.2">
+    <row r="24" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G24" s="15" t="s">
         <v>37</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="7:28" x14ac:dyDescent="0.2">
+    <row r="25" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G25" s="15" t="s">
         <v>38</v>
       </c>
@@ -2009,7 +2009,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="26" spans="7:28" x14ac:dyDescent="0.2">
+    <row r="26" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G26" s="15" t="s">
         <v>39</v>
       </c>
@@ -2059,7 +2059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="7:28" x14ac:dyDescent="0.2">
+    <row r="27" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G27" s="15" t="s">
         <v>40</v>
       </c>
@@ -2109,7 +2109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="7:28" x14ac:dyDescent="0.2">
+    <row r="28" spans="7:28" x14ac:dyDescent="0.25">
       <c r="G28" s="16"/>
       <c r="M28" s="15">
         <f t="shared" ref="M28:R28" si="16">SUM(M5:M27)</f>
@@ -2150,20 +2150,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B32DD369-036A-401E-813F-D05B564CD920}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B24" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="V83" sqref="V83"/>
+    <sheetView zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="M15" sqref="A2:M15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.34765625" customWidth="1"/>
-    <col min="15" max="15" width="22.734375" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="15" max="15" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>60</v>
       </c>
@@ -2171,7 +2171,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
@@ -2199,7 +2199,7 @@
       <c r="V2" s="26"/>
       <c r="W2" s="27"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>54</v>
       </c>
@@ -2267,7 +2267,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
         <v>53</v>
       </c>
@@ -2335,7 +2335,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>44</v>
       </c>
@@ -2403,7 +2403,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>45</v>
       </c>
@@ -2471,7 +2471,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>46</v>
       </c>
@@ -2539,7 +2539,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>55</v>
       </c>
@@ -2607,7 +2607,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>47</v>
       </c>
@@ -2675,7 +2675,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>48</v>
       </c>
@@ -2743,7 +2743,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>49</v>
       </c>
@@ -2811,7 +2811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>50</v>
       </c>
@@ -2879,7 +2879,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>51</v>
       </c>
@@ -2947,7 +2947,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>52</v>
       </c>
@@ -3015,7 +3015,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>56</v>
       </c>
@@ -3083,7 +3083,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
         <v>58</v>
       </c>
@@ -3111,7 +3111,7 @@
       <c r="V17" s="26"/>
       <c r="W17" s="27"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>54</v>
       </c>
@@ -3179,7 +3179,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
         <v>53</v>
       </c>
@@ -3247,7 +3247,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
         <v>59</v>
       </c>
@@ -3315,7 +3315,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
         <v>45</v>
       </c>
@@ -3383,7 +3383,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>46</v>
       </c>
@@ -3451,7 +3451,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>55</v>
       </c>
@@ -3519,7 +3519,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
         <v>47</v>
       </c>
@@ -3587,7 +3587,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>48</v>
       </c>
@@ -3655,7 +3655,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>49</v>
       </c>
@@ -3723,7 +3723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
         <v>50</v>
       </c>
@@ -3791,7 +3791,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="20" t="s">
         <v>51</v>
       </c>
@@ -3859,7 +3859,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>52</v>
       </c>
@@ -3927,7 +3927,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
         <v>56</v>
       </c>
@@ -3995,7 +3995,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="25" t="s">
         <v>62</v>
       </c>
@@ -4023,7 +4023,7 @@
       <c r="V33" s="26"/>
       <c r="W33" s="27"/>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="21" t="s">
         <v>54</v>
       </c>
@@ -4091,7 +4091,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="22" t="s">
         <v>53</v>
       </c>
@@ -4159,7 +4159,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
         <v>65</v>
       </c>
@@ -4227,7 +4227,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
         <v>45</v>
       </c>
@@ -4295,7 +4295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
         <v>46</v>
       </c>
@@ -4363,7 +4363,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39" s="19" t="s">
         <v>66</v>
       </c>
@@ -4431,7 +4431,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40" s="19" t="s">
         <v>55</v>
       </c>
@@ -4499,7 +4499,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
         <v>47</v>
       </c>
@@ -4567,7 +4567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42" s="19" t="s">
         <v>67</v>
       </c>
@@ -4635,7 +4635,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
         <v>48</v>
       </c>
@@ -4703,7 +4703,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44" s="19" t="s">
         <v>49</v>
       </c>
@@ -4771,7 +4771,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A45" s="19" t="s">
         <v>50</v>
       </c>
@@ -4839,7 +4839,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A46" s="20" t="s">
         <v>51</v>
       </c>
@@ -4907,7 +4907,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47" s="20" t="s">
         <v>52</v>
       </c>
@@ -4975,7 +4975,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A48" s="19" t="s">
         <v>56</v>
       </c>
@@ -5043,7 +5043,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A51" s="25" t="s">
         <v>68</v>
       </c>
@@ -5071,7 +5071,7 @@
       <c r="V51" s="26"/>
       <c r="W51" s="27"/>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A52" s="21" t="s">
         <v>54</v>
       </c>
@@ -5139,7 +5139,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A53" s="22" t="s">
         <v>53</v>
       </c>
@@ -5207,7 +5207,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A54" s="19" t="s">
         <v>69</v>
       </c>
@@ -5275,7 +5275,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A55" s="19" t="s">
         <v>45</v>
       </c>
@@ -5343,7 +5343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A56" s="19" t="s">
         <v>46</v>
       </c>
@@ -5411,7 +5411,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A57" s="19" t="s">
         <v>66</v>
       </c>
@@ -5479,7 +5479,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A58" s="19" t="s">
         <v>55</v>
       </c>
@@ -5547,7 +5547,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A59" s="19" t="s">
         <v>47</v>
       </c>
@@ -5615,7 +5615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A60" s="19" t="s">
         <v>67</v>
       </c>
@@ -5683,7 +5683,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A61" s="19" t="s">
         <v>48</v>
       </c>
@@ -5751,7 +5751,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A62" s="19" t="s">
         <v>49</v>
       </c>
@@ -5819,7 +5819,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A63" s="19" t="s">
         <v>50</v>
       </c>
@@ -5887,7 +5887,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A64" s="20" t="s">
         <v>51</v>
       </c>
@@ -5955,7 +5955,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A65" s="20" t="s">
         <v>52</v>
       </c>
@@ -6023,7 +6023,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A66" s="19" t="s">
         <v>56</v>
       </c>
@@ -6091,7 +6091,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A70" s="25" t="s">
         <v>70</v>
       </c>
@@ -6119,7 +6119,7 @@
       <c r="V70" s="26"/>
       <c r="W70" s="27"/>
     </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A71" s="21" t="s">
         <v>54</v>
       </c>
@@ -6187,7 +6187,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A72" s="22" t="s">
         <v>53</v>
       </c>
@@ -6255,7 +6255,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A73" s="19" t="s">
         <v>72</v>
       </c>
@@ -6323,7 +6323,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A74" s="19" t="s">
         <v>45</v>
       </c>
@@ -6391,7 +6391,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A75" s="19" t="s">
         <v>46</v>
       </c>
@@ -6459,7 +6459,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A76" s="19" t="s">
         <v>66</v>
       </c>
@@ -6527,7 +6527,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="77" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A77" s="19" t="s">
         <v>55</v>
       </c>
@@ -6595,7 +6595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A78" s="19" t="s">
         <v>47</v>
       </c>
@@ -6663,7 +6663,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="79" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A79" s="19" t="s">
         <v>67</v>
       </c>
@@ -6731,7 +6731,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="80" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A80" s="19" t="s">
         <v>48</v>
       </c>
@@ -6799,7 +6799,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="81" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A81" s="19" t="s">
         <v>49</v>
       </c>
@@ -6867,7 +6867,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="82" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A82" s="19" t="s">
         <v>50</v>
       </c>
@@ -6935,7 +6935,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="83" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A83" s="20" t="s">
         <v>51</v>
       </c>
@@ -7003,7 +7003,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="84" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A84" s="20" t="s">
         <v>52</v>
       </c>
@@ -7071,7 +7071,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="85" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A85" s="19" t="s">
         <v>56</v>
       </c>
@@ -7141,16 +7141,584 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="O2:W2"/>
+    <mergeCell ref="O17:W17"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A33:M33"/>
+    <mergeCell ref="O33:W33"/>
     <mergeCell ref="A51:M51"/>
     <mergeCell ref="O51:W51"/>
     <mergeCell ref="A70:M70"/>
     <mergeCell ref="O70:W70"/>
     <mergeCell ref="A17:M17"/>
-    <mergeCell ref="O2:W2"/>
-    <mergeCell ref="O17:W17"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A33:M33"/>
-    <mergeCell ref="O33:W33"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:M1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="27"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="21">
+        <v>350</v>
+      </c>
+      <c r="C2" s="21">
+        <v>350</v>
+      </c>
+      <c r="D2" s="21">
+        <v>350</v>
+      </c>
+      <c r="E2" s="21">
+        <v>350</v>
+      </c>
+      <c r="F2" s="21">
+        <v>400</v>
+      </c>
+      <c r="G2" s="21">
+        <v>400</v>
+      </c>
+      <c r="H2" s="21">
+        <v>400</v>
+      </c>
+      <c r="I2" s="21">
+        <v>400</v>
+      </c>
+      <c r="J2" s="21">
+        <v>450</v>
+      </c>
+      <c r="K2" s="21">
+        <v>450</v>
+      </c>
+      <c r="L2" s="21">
+        <v>450</v>
+      </c>
+      <c r="M2" s="21">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="23">
+        <v>5</v>
+      </c>
+      <c r="C3" s="24">
+        <v>10</v>
+      </c>
+      <c r="D3" s="24">
+        <v>15</v>
+      </c>
+      <c r="E3" s="24">
+        <v>20</v>
+      </c>
+      <c r="F3" s="24">
+        <v>5</v>
+      </c>
+      <c r="G3" s="24">
+        <v>10</v>
+      </c>
+      <c r="H3" s="24">
+        <v>15</v>
+      </c>
+      <c r="I3" s="24">
+        <v>20</v>
+      </c>
+      <c r="J3" s="24">
+        <v>5</v>
+      </c>
+      <c r="K3" s="24">
+        <v>10</v>
+      </c>
+      <c r="L3" s="24">
+        <v>15</v>
+      </c>
+      <c r="M3" s="24">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="20">
+        <v>30</v>
+      </c>
+      <c r="C4" s="19">
+        <v>30</v>
+      </c>
+      <c r="D4" s="19">
+        <v>35</v>
+      </c>
+      <c r="E4" s="19">
+        <v>35</v>
+      </c>
+      <c r="F4" s="19">
+        <v>30</v>
+      </c>
+      <c r="G4" s="19">
+        <v>35</v>
+      </c>
+      <c r="H4" s="19">
+        <v>35</v>
+      </c>
+      <c r="I4" s="19">
+        <v>35</v>
+      </c>
+      <c r="J4" s="20">
+        <v>30</v>
+      </c>
+      <c r="K4" s="19">
+        <v>35</v>
+      </c>
+      <c r="L4" s="19">
+        <v>35</v>
+      </c>
+      <c r="M4" s="19">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="20">
+        <v>1.5</v>
+      </c>
+      <c r="C5" s="19">
+        <v>2</v>
+      </c>
+      <c r="D5" s="19">
+        <v>2</v>
+      </c>
+      <c r="E5" s="19">
+        <v>2</v>
+      </c>
+      <c r="F5" s="20">
+        <v>1.5</v>
+      </c>
+      <c r="G5" s="19">
+        <v>2</v>
+      </c>
+      <c r="H5" s="19">
+        <v>2</v>
+      </c>
+      <c r="I5" s="19">
+        <v>2</v>
+      </c>
+      <c r="J5" s="20">
+        <v>1.5</v>
+      </c>
+      <c r="K5" s="19">
+        <v>2</v>
+      </c>
+      <c r="L5" s="19">
+        <v>2</v>
+      </c>
+      <c r="M5" s="19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="20">
+        <v>1</v>
+      </c>
+      <c r="C6" s="19">
+        <v>1.25</v>
+      </c>
+      <c r="D6" s="19">
+        <v>2</v>
+      </c>
+      <c r="E6" s="19">
+        <v>2</v>
+      </c>
+      <c r="F6" s="20">
+        <v>1.25</v>
+      </c>
+      <c r="G6" s="19">
+        <v>1.5</v>
+      </c>
+      <c r="H6" s="19">
+        <v>1.75</v>
+      </c>
+      <c r="I6" s="19">
+        <v>2</v>
+      </c>
+      <c r="J6" s="20">
+        <v>1</v>
+      </c>
+      <c r="K6" s="19">
+        <v>1</v>
+      </c>
+      <c r="L6" s="19">
+        <v>1.75</v>
+      </c>
+      <c r="M6" s="19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="20">
+        <v>0</v>
+      </c>
+      <c r="C7" s="19">
+        <v>0</v>
+      </c>
+      <c r="D7" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="E7" s="19">
+        <v>0</v>
+      </c>
+      <c r="F7" s="20">
+        <v>0</v>
+      </c>
+      <c r="G7" s="19">
+        <v>0</v>
+      </c>
+      <c r="H7" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="I7" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="J7" s="20">
+        <v>0</v>
+      </c>
+      <c r="K7" s="19">
+        <v>0</v>
+      </c>
+      <c r="L7" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="M7" s="19">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="C8" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="D8" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="E8" s="19">
+        <v>1</v>
+      </c>
+      <c r="F8" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="G8" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="H8" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="I8" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="J8" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="K8" s="19">
+        <v>1</v>
+      </c>
+      <c r="L8" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="M8" s="19">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="20">
+        <v>1</v>
+      </c>
+      <c r="C9" s="19">
+        <v>1.25</v>
+      </c>
+      <c r="D9" s="19">
+        <v>1.25</v>
+      </c>
+      <c r="E9" s="19">
+        <v>1.5</v>
+      </c>
+      <c r="F9" s="20">
+        <v>1</v>
+      </c>
+      <c r="G9" s="19">
+        <v>1.25</v>
+      </c>
+      <c r="H9" s="19">
+        <v>1.25</v>
+      </c>
+      <c r="I9" s="19">
+        <v>1.25</v>
+      </c>
+      <c r="J9" s="20">
+        <v>1</v>
+      </c>
+      <c r="K9" s="19">
+        <v>1.25</v>
+      </c>
+      <c r="L9" s="19">
+        <v>1.5</v>
+      </c>
+      <c r="M9" s="19">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="C10" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="E10" s="19">
+        <v>1</v>
+      </c>
+      <c r="F10" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="G10" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="H10" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="I10" s="19">
+        <v>1</v>
+      </c>
+      <c r="J10" s="20">
+        <v>0.75</v>
+      </c>
+      <c r="K10" s="19">
+        <v>1</v>
+      </c>
+      <c r="L10" s="19">
+        <v>1</v>
+      </c>
+      <c r="M10" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="20">
+        <v>250</v>
+      </c>
+      <c r="C11" s="20">
+        <v>250</v>
+      </c>
+      <c r="D11" s="19">
+        <v>275</v>
+      </c>
+      <c r="E11" s="19">
+        <v>300</v>
+      </c>
+      <c r="F11" s="20">
+        <v>250</v>
+      </c>
+      <c r="G11" s="19">
+        <v>275</v>
+      </c>
+      <c r="H11" s="19">
+        <v>275</v>
+      </c>
+      <c r="I11" s="19">
+        <v>275</v>
+      </c>
+      <c r="J11" s="20">
+        <v>250</v>
+      </c>
+      <c r="K11" s="19">
+        <v>275</v>
+      </c>
+      <c r="L11" s="19">
+        <v>275</v>
+      </c>
+      <c r="M11" s="19">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="20">
+        <v>100</v>
+      </c>
+      <c r="C12" s="20">
+        <v>100</v>
+      </c>
+      <c r="D12" s="20">
+        <v>100</v>
+      </c>
+      <c r="E12" s="20">
+        <v>150</v>
+      </c>
+      <c r="F12" s="20">
+        <v>100</v>
+      </c>
+      <c r="G12" s="20">
+        <v>100</v>
+      </c>
+      <c r="H12" s="20">
+        <v>100</v>
+      </c>
+      <c r="I12" s="20">
+        <v>100</v>
+      </c>
+      <c r="J12" s="20">
+        <v>100</v>
+      </c>
+      <c r="K12" s="20">
+        <v>100</v>
+      </c>
+      <c r="L12" s="20">
+        <v>100</v>
+      </c>
+      <c r="M12" s="20">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="19">
+        <v>50</v>
+      </c>
+      <c r="C13" s="19">
+        <v>50</v>
+      </c>
+      <c r="D13" s="19">
+        <v>50</v>
+      </c>
+      <c r="E13" s="19">
+        <v>50</v>
+      </c>
+      <c r="F13" s="19">
+        <v>50</v>
+      </c>
+      <c r="G13" s="19">
+        <v>50</v>
+      </c>
+      <c r="H13" s="19">
+        <v>50</v>
+      </c>
+      <c r="I13" s="19">
+        <v>50</v>
+      </c>
+      <c r="J13" s="19">
+        <v>50</v>
+      </c>
+      <c r="K13" s="19">
+        <v>50</v>
+      </c>
+      <c r="L13" s="19">
+        <v>50</v>
+      </c>
+      <c r="M13" s="19">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="20">
+        <v>0</v>
+      </c>
+      <c r="C14" s="19">
+        <v>0</v>
+      </c>
+      <c r="D14" s="19">
+        <v>50</v>
+      </c>
+      <c r="E14" s="19">
+        <v>50</v>
+      </c>
+      <c r="F14" s="20">
+        <v>0</v>
+      </c>
+      <c r="G14" s="19">
+        <v>50</v>
+      </c>
+      <c r="H14" s="19">
+        <v>50</v>
+      </c>
+      <c r="I14" s="19">
+        <v>50</v>
+      </c>
+      <c r="J14" s="20">
+        <v>0</v>
+      </c>
+      <c r="K14" s="19">
+        <v>0</v>
+      </c>
+      <c r="L14" s="19">
+        <v>50</v>
+      </c>
+      <c r="M14" s="19">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changes made to same pattern as least cost feed formuation goes
</commit_message>
<xml_diff>
--- a/assets/latest data/Fixed formulas-2.xlsx
+++ b/assets/latest data/Fixed formulas-2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2234,8 +2234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W85"/>
   <sheetViews>
-    <sheetView zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection sqref="A1:W85"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7222,16 +7222,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="O2:W2"/>
+    <mergeCell ref="O17:W17"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A33:M33"/>
+    <mergeCell ref="O33:W33"/>
     <mergeCell ref="A51:M51"/>
     <mergeCell ref="O51:W51"/>
     <mergeCell ref="A70:M70"/>
     <mergeCell ref="O70:W70"/>
     <mergeCell ref="A17:M17"/>
-    <mergeCell ref="O2:W2"/>
-    <mergeCell ref="O17:W17"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A33:M33"/>
-    <mergeCell ref="O33:W33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15391,7 +15391,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D21"/>
     </sheetView>
   </sheetViews>

</xml_diff>